<commit_message>
pass all tests: updated test_global_ar6 data
</commit_message>
<xml_diff>
--- a/tests/test_data/test_global_ar6.xlsx
+++ b/tests/test_data/test_global_ar6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kikstra\Documents\GitHub\aneris\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24D0D58-DAF0-4E39-845F-54F465003FB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BF14B6-FC08-49D0-8D94-1AB28EA6652B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="2205" windowWidth="18675" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="2835" windowWidth="18675" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:O16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,31 +692,31 @@
         <v>1.6572805247010121</v>
       </c>
       <c r="G3">
-        <v>1.6572805247010121</v>
+        <v>1.6087177454461821</v>
       </c>
       <c r="H3">
-        <v>1.6572805247010121</v>
+        <v>0.84198382161913488</v>
       </c>
       <c r="I3">
-        <v>1.6572805247010121</v>
+        <v>0.70356873633854655</v>
       </c>
       <c r="J3">
-        <v>1.6572805247010121</v>
+        <v>0.54352160754369827</v>
       </c>
       <c r="K3">
-        <v>1.6572805247010121</v>
+        <v>0.47048532309107638</v>
       </c>
       <c r="L3">
-        <v>1.6572805247010121</v>
+        <v>0.4645704816927323</v>
       </c>
       <c r="M3">
-        <v>1.6572805247010121</v>
+        <v>0.4600073568537259</v>
       </c>
       <c r="N3">
-        <v>1.6572805247010121</v>
+        <v>0.45471034728610848</v>
       </c>
       <c r="O3">
-        <v>1.6572805247010121</v>
+        <v>0.44882962125114989</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -739,31 +739,31 @@
         <v>11.474292549999999</v>
       </c>
       <c r="G4">
-        <v>11.474292549999999</v>
+        <v>11.1380649</v>
       </c>
       <c r="H4">
-        <v>11.474292549999999</v>
+        <v>5.8295312999999984</v>
       </c>
       <c r="I4">
-        <v>11.474292549999999</v>
+        <v>4.8712052000000003</v>
       </c>
       <c r="J4">
-        <v>11.474292549999999</v>
+        <v>3.7631082</v>
       </c>
       <c r="K4">
-        <v>11.474292549999999</v>
+        <v>3.2574366000000001</v>
       </c>
       <c r="L4">
-        <v>11.474292549999999</v>
+        <v>3.2164847999999999</v>
       </c>
       <c r="M4">
-        <v>11.474292549999999</v>
+        <v>3.1848917000000001</v>
       </c>
       <c r="N4">
-        <v>11.474292549999999</v>
+        <v>3.1482174999999999</v>
       </c>
       <c r="O4">
-        <v>11.474292549999999</v>
+        <v>3.1075018999999999</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1021,31 +1021,31 @@
         <v>851.41739683000014</v>
       </c>
       <c r="G10">
-        <v>851.41739683000014</v>
+        <v>1229.7630355010001</v>
       </c>
       <c r="H10">
-        <v>851.41739683000014</v>
+        <v>752.09889483300003</v>
       </c>
       <c r="I10">
-        <v>851.41739683000014</v>
+        <v>911.79343712600019</v>
       </c>
       <c r="J10">
-        <v>851.41739683000014</v>
+        <v>938.14800622400003</v>
       </c>
       <c r="K10">
-        <v>851.41739683000014</v>
+        <v>1014.501330986</v>
       </c>
       <c r="L10">
-        <v>851.41739683000014</v>
+        <v>1040.6988646340001</v>
       </c>
       <c r="M10">
-        <v>851.41739683000014</v>
+        <v>1015.725827259</v>
       </c>
       <c r="N10">
-        <v>851.41739683000014</v>
+        <v>982.03410548100032</v>
       </c>
       <c r="O10">
-        <v>851.41739683000014</v>
+        <v>936.62987589600016</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1068,31 +1068,31 @@
         <v>10900</v>
       </c>
       <c r="G11">
-        <v>10900</v>
+        <v>10715.028417993401</v>
       </c>
       <c r="H11">
-        <v>10900</v>
+        <v>10018.589616762691</v>
       </c>
       <c r="I11">
-        <v>10900</v>
+        <v>9197.7736844025676</v>
       </c>
       <c r="J11">
-        <v>10900</v>
+        <v>8111.9367114782908</v>
       </c>
       <c r="K11">
-        <v>10900</v>
+        <v>7196.2146728144562</v>
       </c>
       <c r="L11">
-        <v>10900</v>
+        <v>6042.0082227535131</v>
       </c>
       <c r="M11">
-        <v>10900</v>
+        <v>5323.6645717810206</v>
       </c>
       <c r="N11">
-        <v>10900</v>
+        <v>4897.5210224890106</v>
       </c>
       <c r="O11">
-        <v>10900</v>
+        <v>4495.4184032751537</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>